<commit_message>
feat: add county code service to api
</commit_message>
<xml_diff>
--- a/testing/country-onbaording.xlsx
+++ b/testing/country-onbaording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_g\lui\fwthompsonjr\leads-ui\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE35AA82-2C93-4812-AFCF-6DAF56E3C434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F48FC90-2718-46B7-8C0F-A7C522557B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{036EAB4B-117B-466D-B077-96206B60865D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{036EAB4B-117B-466D-B077-96206B60865D}"/>
   </bookViews>
   <sheets>
     <sheet name="Counties" sheetId="1" r:id="rId1"/>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86410215-1CBD-4B54-8840-1835B106D5AC}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>